<commit_message>
Log full RTI questions in standardized format
</commit_message>
<xml_diff>
--- a/ESG_Indigenous_Economies_Paper/03_RTI_Tracking/Filed_RTIs.xlsx
+++ b/ESG_Indigenous_Economies_Paper/03_RTI_Tracking/Filed_RTIs.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New folder\ESG\ESG_Indigenous_Economies_Paper\03_RTI_Tracking\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D42FC3-59BA-4966-99DC-1F5E0B6CA0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>RTI ID</t>
   </si>
@@ -35,13 +41,87 @@
   </si>
   <si>
     <t>Action Required</t>
+  </si>
+  <si>
+    <t>RTI2025-TRIFED-02</t>
+  </si>
+  <si>
+    <t>TRIFED (under MoTA)</t>
+  </si>
+  <si>
+    <t>Tribal enterprises, turnover, ESG investments</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Await response</t>
+  </si>
+  <si>
+    <t>RTI2025-MoTA-01</t>
+  </si>
+  <si>
+    <t>Ministry of Tribal Affairs</t>
+  </si>
+  <si>
+    <t>FRA claims, Van Dhan Kendras, tribal cooperatives</t>
+  </si>
+  <si>
+    <t>RTI2025-MCA-03</t>
+  </si>
+  <si>
+    <t>Ministry of Corporate Affairs</t>
+  </si>
+  <si>
+    <t>CSR expenditures, ESG disclosures in tribal districts</t>
+  </si>
+  <si>
+    <t>RTI2025-MoEFCC-04</t>
+  </si>
+  <si>
+    <t>MoEFCC Regional Office Bhopal</t>
+  </si>
+  <si>
+    <t>MFP revenues, CFR governance, tribal forest livelihoods</t>
+  </si>
+  <si>
+    <t>Full Questions Text</t>
+  </si>
+  <si>
+    <t>2025-06-10</t>
+  </si>
+  <si>
+    <t>1. List of Van Dhan Kendras with location nature of products and year of establishment
+2. Annual turnover and profit or loss data of each Kendra
+3. Details of training marketing or value addition support provided to these Kendras
+4. Any record of ESG investment or impact investment in these tribal enterprises
+5. Copies of monitoring or evaluation reports for TRIFED activities in Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>1. District-wise number of Individual Forest Rights and Community Forest Rights claims filed approved and rejected
+2. Forest area in hectares recognized under CFR
+3. List of Van Dhan Vikas Kendras including year of establishment number of tribal beneficiaries and revenue or profit or loss details from 2020 to 2024
+4. List of tribal cooperatives supported by the Ministry along with type of products employment generated and annual revenue if available
+5. Copies of evaluation reports or audits related to tribal enterprises supported by the Ministry or TRIFED in Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>1. List of companies reporting CSR expenditure in tribal districts of Madhya Pradesh
+2. Project wise CSR spending with name of implementing agency and district
+3. List of companies that submitted ESG or BRSR disclosures related to tribal areas or forest areas in Madhya Pradesh
+4. Any available ESG impact assessments submitted by these companies</t>
+  </si>
+  <si>
+    <t>1. District-wise revenue from sale or trade of minor forest produce including tendu leaves mahua chironji and bamboo
+2. Share of this revenue transferred to tribal gatherers or forest rights holders
+3. List of active Joint Forest Management Committees and CFR Committees under your jurisdiction with available performance data
+4. Copies of evaluation or monitoring reports on tribal livelihoods based on forest resources</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,24 +173,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{F4863624-FBD3-4934-8870-00C22511D24F}"/>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -148,7 +241,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -182,6 +275,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -216,9 +310,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -391,14 +486,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,9 +526,114 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{89db4e91-bad5-4fd0-9ca4-c06485916e3a}" enabled="1" method="Standard" siteId="{f66fae02-5d36-495b-bfe0-78a6ff9f8e6e}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>